<commit_message>
Fixed Neumann function, correct graphing
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanpalmer/Documents/GitHub/HW4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5E432FB-D97E-6D4B-A818-5A07BA538826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C07E357-0FEB-6D41-AE8F-1578B760E1D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17540" xr2:uid="{179D3818-036B-4C42-86FB-148B93EB64D5}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="28040" windowHeight="17540" xr2:uid="{179D3818-036B-4C42-86FB-148B93EB64D5}"/>
   </bookViews>
   <sheets>
     <sheet name="K = 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Nodes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>N = 10</t>
   </si>
@@ -44,7 +41,19 @@
     <t>N = 20</t>
   </si>
   <si>
-    <t>N = 40</t>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>ErrorN</t>
+  </si>
+  <si>
+    <t>Error2N</t>
+  </si>
+  <si>
+    <t>Order of Accuracy</t>
   </si>
 </sst>
 </file>
@@ -396,353 +405,461 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF23F34-F9A9-C64C-8411-47B30C45A47E}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0.84670000000000001</v>
+        <f>1*1/20</f>
+        <v>0.05</v>
       </c>
       <c r="C2">
         <v>0.91769999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>((SINH(1-A2)+SINH(A2))/SINH(1)-1)+(SINH(1-A2)/SINH(1))</f>
+        <v>0.91370591177314542</v>
+      </c>
+      <c r="F2">
+        <f>ABS(C2-D2)</f>
+        <v>3.9940882268545419E-3</v>
+      </c>
+      <c r="G2">
+        <f>LOG(E22/F22)/LOG(2)</f>
+        <v>0.96628860690629981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <f>A2+1*1/20</f>
+        <v>0.1</v>
       </c>
       <c r="B3">
-        <v>0.7087</v>
+        <v>0.84670000000000001</v>
       </c>
       <c r="C3">
         <v>0.83979999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f t="shared" ref="D3:D21" si="0">((SINH(1-A3)+SINH(A3))/SINH(1)-1)+(SINH(1-A3)/SINH(1))</f>
+        <v>0.8321970851306173</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:F22" si="1">ABS(B3-D3)</f>
+        <v>1.450291486938271E-2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F21" si="2">ABS(C3-D3)</f>
+        <v>7.6029148693826931E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.58479999999999999</v>
+        <f t="shared" ref="A4:A20" si="3">A3+1*1/20</f>
+        <v>0.15000000000000002</v>
       </c>
       <c r="C4">
         <v>0.76600000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.75526970554975592</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>1.0730294450244093E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f>A4+1</f>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="B5">
-        <v>0.47399999999999998</v>
+        <v>0.7087</v>
       </c>
       <c r="C5">
         <v>0.69620000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.68273141451192809</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2.5968585488071905E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>1.3468585488071949E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f t="shared" ref="A6:A41" si="0">A5+1</f>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0.37530000000000002</v>
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="C6">
         <v>0.63029999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.61440082850602995</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>1.5899171493970021E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>0.3</v>
       </c>
       <c r="B7">
-        <v>0.28810000000000002</v>
+        <v>0.58479999999999999</v>
       </c>
       <c r="C7">
         <v>0.56810000000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.55010708547523457</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>3.4692914524765417E-2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>1.799291452476548E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.21149999999999999</v>
+        <f t="shared" si="3"/>
+        <v>0.35</v>
       </c>
       <c r="C8">
         <v>0.50939999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.48968941757284978</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1.9710582427150181E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>0.39999999999999997</v>
       </c>
       <c r="B9">
-        <v>0.1449</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="C9">
         <v>0.45419999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.43299674915896114</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>4.1003250841038841E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>2.1203250841038856E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>8.77E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.44999999999999996</v>
       </c>
       <c r="C10">
         <v>0.4022</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.37988731903264233</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>2.2312680967357668E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>0.49999999999999994</v>
       </c>
       <c r="B11">
-        <v>3.9600000000000003E-2</v>
+        <v>0.37530000000000002</v>
       </c>
       <c r="C11">
         <v>0.35349999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.33022832595511081</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>4.5071674044889209E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>2.3271674044889168E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="3"/>
+        <v>0.54999999999999993</v>
       </c>
       <c r="C12">
         <v>0.30780000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.28389559657745878</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>2.3904403422541243E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="B13">
+        <v>0.28810000000000002</v>
       </c>
       <c r="C13">
         <v>0.2651</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.24077327494260015</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>4.7326725057399877E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>2.4326725057399856E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f t="shared" si="3"/>
+        <v>0.65</v>
       </c>
       <c r="C14">
         <v>0.22520000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.20075353278503455</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>2.4446467214965462E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f t="shared" si="3"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="B15">
+        <v>0.21149999999999999</v>
       </c>
       <c r="C15">
         <v>0.18809999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.1637362999040145</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>4.776370009598549E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>2.4363700095985485E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>0.75000000000000011</v>
       </c>
       <c r="C16">
         <v>0.1537</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.1296290139359226</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>2.4070986064077399E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f t="shared" si="3"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="B17">
+        <v>0.1449</v>
       </c>
       <c r="C17">
         <v>0.12189999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>9.8346388900146214E-2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>4.6553611099853787E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>2.355361109985378E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f t="shared" si="3"/>
+        <v>0.8500000000000002</v>
       </c>
       <c r="C18">
         <v>9.2700000000000005E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>6.9810201939704802E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>2.2889798060295202E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="B19">
+        <v>8.77E-2</v>
       </c>
       <c r="C19">
         <v>6.6000000000000003E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>4.3949097723360975E-2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>4.3750902276639025E-2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>2.2050902276639028E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f t="shared" si="3"/>
+        <v>0.95000000000000029</v>
       </c>
       <c r="C20">
         <v>4.1599999999999998E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>2.0698410020126068E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>2.090158997987393E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>3.9600000000000003E-2</v>
       </c>
       <c r="C21">
         <v>1.9699999999999999E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>40</v>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1.9699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <f>MAX(E3:E21)</f>
+        <v>4.776370009598549E-2</v>
+      </c>
+      <c r="F22">
+        <f>MAX(F2:F21)</f>
+        <v>2.4446467214965462E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>